<commit_message>
new diffusion data, new membrane video
</commit_message>
<xml_diff>
--- a/sheet05/data/argon_diffusion.xlsx
+++ b/sheet05/data/argon_diffusion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\tobias\MolSimPresentation\sheet05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9C0C61-751A-481E-95FA-3872F1DAEF00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BAE070-665C-4857-9F26-3B4CD0D75154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Diffusion History</a:t>
+              <a:t>Diffusion History (Sampled every 2500 Iterations)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -525,304 +525,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="103"/>
                 <c:pt idx="0">
-                  <c:v>11.5823</c:v>
+                  <c:v>4.8048799999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.4145</c:v>
+                  <c:v>4.6066000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.6343</c:v>
+                  <c:v>5.0177800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.3245</c:v>
+                  <c:v>4.1695500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.9613</c:v>
+                  <c:v>4.4600999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.443199999999999</c:v>
+                  <c:v>4.29209</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.8302800000000001</c:v>
+                  <c:v>4.4374700000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.4221</c:v>
+                  <c:v>4.6578099999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3645399999999999</c:v>
+                  <c:v>4.1711999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.513</c:v>
+                  <c:v>3.9134600000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.014699999999999</c:v>
+                  <c:v>4.1370800000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.8689999999999998</c:v>
+                  <c:v>4.3628799999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.1074</c:v>
+                  <c:v>4.09361</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10.1341</c:v>
+                  <c:v>4.1980700000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.3924199999999995</c:v>
+                  <c:v>4.0887500000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.5673700000000004</c:v>
+                  <c:v>3.83996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.595599999999999</c:v>
+                  <c:v>4.0241699999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.4558</c:v>
+                  <c:v>3.7074799999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.1355</c:v>
+                  <c:v>3.69801</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9747599999999998</c:v>
+                  <c:v>4.4468800000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.9314199999999992</c:v>
+                  <c:v>3.5792799999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.6961399999999998</c:v>
+                  <c:v>3.6743000000000001</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.7101000000000006</c:v>
+                  <c:v>3.8503500000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>10.167899999999999</c:v>
+                  <c:v>3.99356</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.6303300000000007</c:v>
+                  <c:v>3.6864599999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.2806800000000003</c:v>
+                  <c:v>3.38</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.3581500000000002</c:v>
+                  <c:v>3.2318899999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9.5180500000000006</c:v>
+                  <c:v>3.3169200000000001</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.7977500000000006</c:v>
+                  <c:v>3.7360099999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.6133000000000006</c:v>
+                  <c:v>3.3249399999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>8.6107700000000005</c:v>
+                  <c:v>3.1988500000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>8.2163599999999999</c:v>
+                  <c:v>3.2259099999999998</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.3551099999999998</c:v>
+                  <c:v>3.1590799999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.8059399999999997</c:v>
+                  <c:v>3.2181600000000001</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.2810000000000006</c:v>
+                  <c:v>3.02874</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>7.9122899999999996</c:v>
+                  <c:v>3.2555999999999998</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.7237100000000005</c:v>
+                  <c:v>3.10263</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.3491900000000001</c:v>
+                  <c:v>2.9090099999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.7038099999999998</c:v>
+                  <c:v>3.0103300000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.2657999999999996</c:v>
+                  <c:v>2.8391199999999999</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.3569700000000005</c:v>
+                  <c:v>2.90306</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>8.1071600000000004</c:v>
+                  <c:v>2.6816900000000001</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.9393500000000001</c:v>
+                  <c:v>2.72397</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.6155299999999997</c:v>
+                  <c:v>2.9557199999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.80877</c:v>
+                  <c:v>2.5720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.3679800000000002</c:v>
+                  <c:v>2.48515</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8.12791</c:v>
+                  <c:v>2.5375000000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.2869099999999998</c:v>
+                  <c:v>2.3976899999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>7.8736699999999997</c:v>
+                  <c:v>2.6780499999999998</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.9713799999999999</c:v>
+                  <c:v>2.5420199999999999</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.5320600000000004</c:v>
+                  <c:v>2.4811999999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.5980499999999997</c:v>
+                  <c:v>2.3658199999999998</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7.2129799999999999</c:v>
+                  <c:v>2.41214</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7.0805899999999999</c:v>
+                  <c:v>2.5205600000000001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6.7166199999999998</c:v>
+                  <c:v>2.2610299999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>7.6000500000000004</c:v>
+                  <c:v>2.3469600000000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7.0628900000000003</c:v>
+                  <c:v>2.2210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7.0819200000000002</c:v>
+                  <c:v>1.9353199999999999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6.9360799999999996</c:v>
+                  <c:v>2.0588500000000001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.9888899999999996</c:v>
+                  <c:v>2.0888</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.2000900000000003</c:v>
+                  <c:v>1.9130199999999999</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6.8265399999999996</c:v>
+                  <c:v>1.7782100000000001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.1270600000000002</c:v>
+                  <c:v>1.8512999999999999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.1308499999999997</c:v>
+                  <c:v>1.67974</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.2979000000000003</c:v>
+                  <c:v>1.82142</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.2078199999999999</c:v>
+                  <c:v>1.7111700000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.1746299999999996</c:v>
+                  <c:v>1.85869</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>6.3601999999999999</c:v>
+                  <c:v>1.77458</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.9301500000000003</c:v>
+                  <c:v>1.64882</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.5186099999999998</c:v>
+                  <c:v>1.5088999999999999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6.1236899999999999</c:v>
+                  <c:v>1.5301800000000001</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.39018</c:v>
+                  <c:v>1.3187899999999999</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>6.0289400000000004</c:v>
+                  <c:v>1.4168499999999999</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.5792799999999998</c:v>
+                  <c:v>1.2976099999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.5284700000000004</c:v>
+                  <c:v>1.28661</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5.8122100000000003</c:v>
+                  <c:v>1.22272</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.1693800000000003</c:v>
+                  <c:v>1.2784</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.3819499999999998</c:v>
+                  <c:v>1.2839</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.6578600000000003</c:v>
+                  <c:v>1.18347</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.0157299999999996</c:v>
+                  <c:v>1.04802</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.7200199999999999</c:v>
+                  <c:v>1.05664</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.7538799999999997</c:v>
+                  <c:v>0.96916599999999997</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.8214100000000002</c:v>
+                  <c:v>0.96930899999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.0613299999999999</c:v>
+                  <c:v>0.90728799999999998</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.0863199999999997</c:v>
+                  <c:v>0.83740199999999998</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>3.9412799999999999</c:v>
+                  <c:v>0.80911200000000005</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.2573699999999999</c:v>
+                  <c:v>0.66082200000000002</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.5664999999999996</c:v>
+                  <c:v>0.65816300000000005</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.9846699999999999</c:v>
+                  <c:v>0.665107</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.2580799999999996</c:v>
+                  <c:v>0.65404200000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>3.9935299999999998</c:v>
+                  <c:v>0.599074</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3.2849699999999999</c:v>
+                  <c:v>0.53460099999999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>3.2231200000000002</c:v>
+                  <c:v>0.51446999999999998</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.5000499999999999</c:v>
+                  <c:v>0.485211</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.3731499999999999</c:v>
+                  <c:v>0.46825600000000001</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3.1986400000000001</c:v>
+                  <c:v>0.45920100000000003</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.5594399999999999</c:v>
+                  <c:v>0.43281799999999998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.6231599999999999</c:v>
+                  <c:v>0.42285400000000001</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.82626</c:v>
+                  <c:v>0.432861</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>3.7863099999999998</c:v>
+                  <c:v>0.38176700000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1184,304 +1184,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>11.1097</c:v>
+                  <c:v>4.6291200000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.6638</c:v>
+                  <c:v>4.3482799999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.4935500000000008</c:v>
+                  <c:v>4.2432999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6340599999999998</c:v>
+                  <c:v>3.7139799999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6563999999999997</c:v>
+                  <c:v>3.6131099999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.218400000000001</c:v>
+                  <c:v>3.0177499999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.7793799999999997</c:v>
+                  <c:v>2.8149700000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9545300000000001</c:v>
+                  <c:v>2.3936700000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.35806</c:v>
+                  <c:v>2.28592</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8679399999999999</c:v>
+                  <c:v>1.83944</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.5255400000000003</c:v>
+                  <c:v>1.69072</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0403799999999999</c:v>
+                  <c:v>1.36771</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9756200000000002</c:v>
+                  <c:v>1.0199400000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.4317799999999998</c:v>
+                  <c:v>0.81782699999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.20166</c:v>
+                  <c:v>0.55414600000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7781400000000001</c:v>
+                  <c:v>0.36572300000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1056499999999998</c:v>
+                  <c:v>0.239847</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6729000000000001</c:v>
+                  <c:v>0.12856699999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.86271500000000001</c:v>
+                  <c:v>6.7912799999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.85130099999999997</c:v>
+                  <c:v>2.9829899999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.67776099999999995</c:v>
+                  <c:v>1.6630200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.181362</c:v>
+                  <c:v>3.1474799999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.4508099999999999E-2</c:v>
+                  <c:v>2.0897900000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.33586300000000002</c:v>
+                  <c:v>1.71475E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.50048700000000002</c:v>
+                  <c:v>1.9549199999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.165156</c:v>
+                  <c:v>2.0939300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.66290000000000004</c:v>
+                  <c:v>1.1652300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.50619000000000003</c:v>
+                  <c:v>1.1517100000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.65239499999999995</c:v>
+                  <c:v>7.3006299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.33361800000000003</c:v>
+                  <c:v>4.5135599999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.33196900000000001</c:v>
+                  <c:v>3.3561300000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.33645900000000001</c:v>
+                  <c:v>4.1259599999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.16762299999999999</c:v>
+                  <c:v>2.5538900000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.66162900000000002</c:v>
+                  <c:v>2.1857000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99140200000000001</c:v>
+                  <c:v>2.4963400000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.49589800000000001</c:v>
+                  <c:v>2.3074200000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.49598999999999999</c:v>
+                  <c:v>2.0121599999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.166881</c:v>
+                  <c:v>2.5523500000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.33084599999999997</c:v>
+                  <c:v>2.5428600000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.16711000000000001</c:v>
+                  <c:v>2.4356500000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.33131500000000003</c:v>
+                  <c:v>1.6373200000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.16605300000000001</c:v>
+                  <c:v>1.5728599999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.329127</c:v>
+                  <c:v>1.4586499999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.2952900000000002E-3</c:v>
+                  <c:v>1.61342E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.9983000000000002E-3</c:v>
+                  <c:v>1.5826600000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.167237</c:v>
+                  <c:v>1.90087E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.16658200000000001</c:v>
+                  <c:v>1.7228899999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.65893199999999996</c:v>
+                  <c:v>1.56521E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.33021699999999998</c:v>
+                  <c:v>2.5086499999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.65660499999999999</c:v>
+                  <c:v>1.92275E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.49215199999999998</c:v>
+                  <c:v>1.5084E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.32714500000000002</c:v>
+                  <c:v>2.24033E-3</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.16597100000000001</c:v>
+                  <c:v>2.2804499999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.49537700000000001</c:v>
+                  <c:v>1.9222200000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.65753099999999998</c:v>
+                  <c:v>2.4226299999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.33002100000000001</c:v>
+                  <c:v>2.0982599999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.16636500000000001</c:v>
+                  <c:v>2.51447E-3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.166239</c:v>
+                  <c:v>3.1665299999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.16597300000000001</c:v>
+                  <c:v>2.36901E-3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.49503799999999998</c:v>
+                  <c:v>2.1789999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.65898100000000004</c:v>
+                  <c:v>2.2827199999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.166986</c:v>
+                  <c:v>1.81237E-3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.49584800000000001</c:v>
+                  <c:v>2.2105900000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.66056099999999995</c:v>
+                  <c:v>1.9303E-3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.330596</c:v>
+                  <c:v>3.2170499999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.75505E-3</c:v>
+                  <c:v>3.2174299999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.16536600000000001</c:v>
+                  <c:v>3.24924E-3</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.32932400000000001</c:v>
+                  <c:v>2.3193300000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.49462</c:v>
+                  <c:v>2.5328600000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.495284</c:v>
+                  <c:v>2.1566799999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.16603799999999999</c:v>
+                  <c:v>2.3112900000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.329621</c:v>
+                  <c:v>1.7953999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.49267</c:v>
+                  <c:v>2.25961E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.81939799999999996</c:v>
+                  <c:v>1.8689100000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.65917199999999998</c:v>
+                  <c:v>1.90693E-3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.81967400000000001</c:v>
+                  <c:v>2.1695E-3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.49275600000000003</c:v>
+                  <c:v>2.1294600000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.82478099999999999</c:v>
+                  <c:v>1.8750699999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.495305</c:v>
+                  <c:v>1.8830400000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.65873700000000002</c:v>
+                  <c:v>1.94173E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.32969599999999999</c:v>
+                  <c:v>2.0902899999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.49456800000000001</c:v>
+                  <c:v>3.0154499999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.33023000000000002</c:v>
+                  <c:v>1.85227E-3</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.49491099999999999</c:v>
+                  <c:v>1.81492E-3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.33126299999999997</c:v>
+                  <c:v>2.1383399999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.33006999999999997</c:v>
+                  <c:v>3.6200799999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.328851</c:v>
+                  <c:v>3.4783399999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.329291</c:v>
+                  <c:v>3.00038E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.49656600000000001</c:v>
+                  <c:v>2.2781799999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.16579199999999999</c:v>
+                  <c:v>3.8428799999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.330507</c:v>
+                  <c:v>4.5530900000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.65519099999999997</c:v>
+                  <c:v>2.6874500000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.327984</c:v>
+                  <c:v>3.01308E-3</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.32834600000000003</c:v>
+                  <c:v>2.4972800000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.32916499999999999</c:v>
+                  <c:v>2.1240199999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.49386400000000003</c:v>
+                  <c:v>2.0739600000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.49198599999999998</c:v>
+                  <c:v>2.3248100000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.165939</c:v>
+                  <c:v>2.6210199999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.330571</c:v>
+                  <c:v>3.06558E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.16677500000000001</c:v>
+                  <c:v>3.01951E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2442,11 +2442,11 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.19201</cdr:x>
-      <cdr:y>0.51288</cdr:y>
+      <cdr:x>0.18601</cdr:x>
+      <cdr:y>0.6313</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.19201</cdr:x>
+      <cdr:x>0.18601</cdr:x>
       <cdr:y>0.78302</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -2462,8 +2462,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="1172307" y="2031023"/>
-          <a:ext cx="0" cy="1069731"/>
+          <a:off x="1135653" y="2499946"/>
+          <a:ext cx="0" cy="600813"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -2495,11 +2495,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.72485</cdr:x>
-      <cdr:y>0.55174</cdr:y>
+      <cdr:x>0.72125</cdr:x>
+      <cdr:y>0.63315</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.72485</cdr:x>
+      <cdr:x>0.72125</cdr:x>
       <cdr:y>0.78302</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
@@ -2515,8 +2515,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="4425461" y="2184888"/>
-          <a:ext cx="0" cy="915866"/>
+          <a:off x="4403479" y="2507273"/>
+          <a:ext cx="0" cy="593486"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -2548,12 +2548,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.15713</cdr:x>
-      <cdr:y>0.78623</cdr:y>
+      <cdr:x>0.14753</cdr:x>
+      <cdr:y>0.78993</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.22467</cdr:x>
-      <cdr:y>0.84786</cdr:y>
+      <cdr:x>0.21507</cdr:x>
+      <cdr:y>0.85156</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2568,8 +2568,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="959338" y="3113454"/>
-          <a:ext cx="412357" cy="244078"/>
+          <a:off x="900717" y="3128125"/>
+          <a:ext cx="412355" cy="244055"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2757,6 +2757,120 @@
         </a:p>
       </cdr:txBody>
     </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61204</cdr:x>
+      <cdr:y>0.13174</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.93486</cdr:x>
+      <cdr:y>0.32601</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="11" name="Textfeld 10">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BF3EF86-01BA-FA2B-7141-C78F70E62523}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3736730" y="521677"/>
+          <a:ext cx="1970942" cy="769327"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 31125"/>
+          </a:avLst>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="2">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </cdr:style>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Additional timestamps</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> show when boiling point temperature is reached</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.08401</cdr:x>
+      <cdr:y>0.63062</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.94687</cdr:x>
+      <cdr:y>0.63062</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="13" name="Gerader Verbinder 12">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E12C3A3F-9F7F-F2D1-621C-41FFE202405D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="512884" y="2497252"/>
+          <a:ext cx="5268058" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
   </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
@@ -3027,7 +3141,7 @@
   <dimension ref="C2:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="T2" sqref="T2:T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3059,13 +3173,13 @@
         <v>2500</v>
       </c>
       <c r="D4">
-        <v>11.5823</v>
+        <v>4.8048799999999998</v>
       </c>
       <c r="E4">
         <v>2500</v>
       </c>
       <c r="F4">
-        <v>11.1097</v>
+        <v>4.6291200000000003</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
@@ -3073,13 +3187,13 @@
         <v>5000</v>
       </c>
       <c r="D5">
-        <v>11.4145</v>
+        <v>4.6066000000000003</v>
       </c>
       <c r="E5">
         <v>5000</v>
       </c>
       <c r="F5">
-        <v>10.6638</v>
+        <v>4.3482799999999999</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
@@ -3087,13 +3201,13 @@
         <v>7500</v>
       </c>
       <c r="D6">
-        <v>10.6343</v>
+        <v>5.0177800000000001</v>
       </c>
       <c r="E6">
         <v>7500</v>
       </c>
       <c r="F6">
-        <v>9.4935500000000008</v>
+        <v>4.2432999999999996</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
@@ -3101,13 +3215,13 @@
         <v>10000</v>
       </c>
       <c r="D7">
-        <v>11.3245</v>
+        <v>4.1695500000000001</v>
       </c>
       <c r="E7">
         <v>10000</v>
       </c>
       <c r="F7">
-        <v>8.6340599999999998</v>
+        <v>3.7139799999999998</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
@@ -3115,13 +3229,13 @@
         <v>12500</v>
       </c>
       <c r="D8">
-        <v>10.9613</v>
+        <v>4.4600999999999997</v>
       </c>
       <c r="E8">
         <v>12500</v>
       </c>
       <c r="F8">
-        <v>8.6563999999999997</v>
+        <v>3.6131099999999998</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
@@ -3129,13 +3243,13 @@
         <v>15000</v>
       </c>
       <c r="D9">
-        <v>10.443199999999999</v>
+        <v>4.29209</v>
       </c>
       <c r="E9">
         <v>15000</v>
       </c>
       <c r="F9">
-        <v>10.218400000000001</v>
+        <v>3.0177499999999999</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
@@ -3143,13 +3257,13 @@
         <v>17500</v>
       </c>
       <c r="D10">
-        <v>9.8302800000000001</v>
+        <v>4.4374700000000002</v>
       </c>
       <c r="E10">
         <v>17500</v>
       </c>
       <c r="F10">
-        <v>7.7793799999999997</v>
+        <v>2.8149700000000002</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
@@ -3157,13 +3271,13 @@
         <v>20000</v>
       </c>
       <c r="D11">
-        <v>10.4221</v>
+        <v>4.6578099999999996</v>
       </c>
       <c r="E11">
         <v>20000</v>
       </c>
       <c r="F11">
-        <v>7.9545300000000001</v>
+        <v>2.3936700000000002</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
@@ -3171,13 +3285,13 @@
         <v>22500</v>
       </c>
       <c r="D12">
-        <v>9.3645399999999999</v>
+        <v>4.1711999999999998</v>
       </c>
       <c r="E12">
         <v>22500</v>
       </c>
       <c r="F12">
-        <v>7.35806</v>
+        <v>2.28592</v>
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
@@ -3185,13 +3299,13 @@
         <v>25000</v>
       </c>
       <c r="D13">
-        <v>10.513</v>
+        <v>3.9134600000000002</v>
       </c>
       <c r="E13">
         <v>25000</v>
       </c>
       <c r="F13">
-        <v>5.8679399999999999</v>
+        <v>1.83944</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
@@ -3199,13 +3313,13 @@
         <v>27500</v>
       </c>
       <c r="D14">
-        <v>11.014699999999999</v>
+        <v>4.1370800000000001</v>
       </c>
       <c r="E14">
         <v>27500</v>
       </c>
       <c r="F14">
-        <v>6.5255400000000003</v>
+        <v>1.69072</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
@@ -3213,13 +3327,13 @@
         <v>30000</v>
       </c>
       <c r="D15">
-        <v>9.8689999999999998</v>
+        <v>4.3628799999999996</v>
       </c>
       <c r="E15">
         <v>30000</v>
       </c>
       <c r="F15">
-        <v>5.0403799999999999</v>
+        <v>1.36771</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
@@ -3227,13 +3341,13 @@
         <v>32500</v>
       </c>
       <c r="D16">
-        <v>11.1074</v>
+        <v>4.09361</v>
       </c>
       <c r="E16">
         <v>32500</v>
       </c>
       <c r="F16">
-        <v>5.9756200000000002</v>
+        <v>1.0199400000000001</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -3241,13 +3355,13 @@
         <v>35000</v>
       </c>
       <c r="D17">
-        <v>10.1341</v>
+        <v>4.1980700000000004</v>
       </c>
       <c r="E17">
         <v>35000</v>
       </c>
       <c r="F17">
-        <v>5.4317799999999998</v>
+        <v>0.81782699999999997</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -3255,13 +3369,13 @@
         <v>37500</v>
       </c>
       <c r="D18">
-        <v>9.3924199999999995</v>
+        <v>4.0887500000000001</v>
       </c>
       <c r="E18">
         <v>37500</v>
       </c>
       <c r="F18">
-        <v>3.20166</v>
+        <v>0.55414600000000003</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
@@ -3269,13 +3383,13 @@
         <v>40000</v>
       </c>
       <c r="D19">
-        <v>9.5673700000000004</v>
+        <v>3.83996</v>
       </c>
       <c r="E19">
         <v>40000</v>
       </c>
       <c r="F19">
-        <v>2.7781400000000001</v>
+        <v>0.36572300000000002</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
@@ -3283,13 +3397,13 @@
         <v>42500</v>
       </c>
       <c r="D20">
-        <v>11.595599999999999</v>
+        <v>4.0241699999999998</v>
       </c>
       <c r="E20">
         <v>42500</v>
       </c>
       <c r="F20">
-        <v>2.1056499999999998</v>
+        <v>0.239847</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -3297,13 +3411,13 @@
         <v>45000</v>
       </c>
       <c r="D21">
-        <v>10.4558</v>
+        <v>3.7074799999999999</v>
       </c>
       <c r="E21">
         <v>45000</v>
       </c>
       <c r="F21">
-        <v>1.6729000000000001</v>
+        <v>0.12856699999999999</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -3311,13 +3425,13 @@
         <v>47500</v>
       </c>
       <c r="D22">
-        <v>10.1355</v>
+        <v>3.69801</v>
       </c>
       <c r="E22">
         <v>47500</v>
       </c>
       <c r="F22">
-        <v>0.86271500000000001</v>
+        <v>6.7912799999999995E-2</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
@@ -3325,13 +3439,13 @@
         <v>50000</v>
       </c>
       <c r="D23">
-        <v>8.9747599999999998</v>
+        <v>4.4468800000000002</v>
       </c>
       <c r="E23">
         <v>50000</v>
       </c>
       <c r="F23">
-        <v>0.85130099999999997</v>
+        <v>2.9829899999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
@@ -3339,13 +3453,13 @@
         <v>52500</v>
       </c>
       <c r="D24">
-        <v>9.9314199999999992</v>
+        <v>3.5792799999999998</v>
       </c>
       <c r="E24">
         <v>52500</v>
       </c>
       <c r="F24">
-        <v>0.67776099999999995</v>
+        <v>1.6630200000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
@@ -3353,13 +3467,13 @@
         <v>55000</v>
       </c>
       <c r="D25">
-        <v>9.6961399999999998</v>
+        <v>3.6743000000000001</v>
       </c>
       <c r="E25">
         <v>55000</v>
       </c>
       <c r="F25">
-        <v>0.181362</v>
+        <v>3.1474799999999997E-2</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
@@ -3367,13 +3481,13 @@
         <v>57500</v>
       </c>
       <c r="D26">
-        <v>8.7101000000000006</v>
+        <v>3.8503500000000002</v>
       </c>
       <c r="E26">
         <v>57500</v>
       </c>
       <c r="F26">
-        <v>1.4508099999999999E-2</v>
+        <v>2.0897900000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
@@ -3381,13 +3495,13 @@
         <v>60000</v>
       </c>
       <c r="D27">
-        <v>10.167899999999999</v>
+        <v>3.99356</v>
       </c>
       <c r="E27">
         <v>60000</v>
       </c>
       <c r="F27">
-        <v>0.33586300000000002</v>
+        <v>1.71475E-2</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
@@ -3395,13 +3509,13 @@
         <v>62500</v>
       </c>
       <c r="D28">
-        <v>8.6303300000000007</v>
+        <v>3.6864599999999998</v>
       </c>
       <c r="E28">
         <v>62500</v>
       </c>
       <c r="F28">
-        <v>0.50048700000000002</v>
+        <v>1.9549199999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
@@ -3409,13 +3523,13 @@
         <v>65000</v>
       </c>
       <c r="D29">
-        <v>9.2806800000000003</v>
+        <v>3.38</v>
       </c>
       <c r="E29">
         <v>65000</v>
       </c>
       <c r="F29">
-        <v>0.165156</v>
+        <v>2.0939300000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
@@ -3423,13 +3537,13 @@
         <v>67500</v>
       </c>
       <c r="D30">
-        <v>9.3581500000000002</v>
+        <v>3.2318899999999999</v>
       </c>
       <c r="E30">
         <v>67500</v>
       </c>
       <c r="F30">
-        <v>0.66290000000000004</v>
+        <v>1.1652300000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
@@ -3437,13 +3551,13 @@
         <v>70000</v>
       </c>
       <c r="D31">
-        <v>9.5180500000000006</v>
+        <v>3.3169200000000001</v>
       </c>
       <c r="E31">
         <v>70000</v>
       </c>
       <c r="F31">
-        <v>0.50619000000000003</v>
+        <v>1.1517100000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
@@ -3451,13 +3565,13 @@
         <v>72500</v>
       </c>
       <c r="D32">
-        <v>8.7977500000000006</v>
+        <v>3.7360099999999998</v>
       </c>
       <c r="E32">
         <v>72500</v>
       </c>
       <c r="F32">
-        <v>0.65239499999999995</v>
+        <v>7.3006299999999998E-3</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
@@ -3465,13 +3579,13 @@
         <v>75000</v>
       </c>
       <c r="D33">
-        <v>8.6133000000000006</v>
+        <v>3.3249399999999998</v>
       </c>
       <c r="E33">
         <v>75000</v>
       </c>
       <c r="F33">
-        <v>0.33361800000000003</v>
+        <v>4.5135599999999998E-3</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
@@ -3479,13 +3593,13 @@
         <v>77500</v>
       </c>
       <c r="D34">
-        <v>8.6107700000000005</v>
+        <v>3.1988500000000002</v>
       </c>
       <c r="E34">
         <v>77500</v>
       </c>
       <c r="F34">
-        <v>0.33196900000000001</v>
+        <v>3.3561300000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -3493,13 +3607,13 @@
         <v>80000</v>
       </c>
       <c r="D35">
-        <v>8.2163599999999999</v>
+        <v>3.2259099999999998</v>
       </c>
       <c r="E35">
         <v>80000</v>
       </c>
       <c r="F35">
-        <v>0.33645900000000001</v>
+        <v>4.1259599999999997E-3</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
@@ -3507,13 +3621,13 @@
         <v>82500</v>
       </c>
       <c r="D36">
-        <v>9.3551099999999998</v>
+        <v>3.1590799999999999</v>
       </c>
       <c r="E36">
         <v>82500</v>
       </c>
       <c r="F36">
-        <v>0.16762299999999999</v>
+        <v>2.5538900000000001E-3</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
@@ -3521,13 +3635,13 @@
         <v>85000</v>
       </c>
       <c r="D37">
-        <v>8.8059399999999997</v>
+        <v>3.2181600000000001</v>
       </c>
       <c r="E37">
         <v>85000</v>
       </c>
       <c r="F37">
-        <v>0.66162900000000002</v>
+        <v>2.1857000000000001E-3</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
@@ -3535,13 +3649,13 @@
         <v>87500</v>
       </c>
       <c r="D38">
-        <v>8.2810000000000006</v>
+        <v>3.02874</v>
       </c>
       <c r="E38">
         <v>87500</v>
       </c>
       <c r="F38">
-        <v>0.99140200000000001</v>
+        <v>2.4963400000000001E-3</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
@@ -3549,13 +3663,13 @@
         <v>90000</v>
       </c>
       <c r="D39">
-        <v>7.9122899999999996</v>
+        <v>3.2555999999999998</v>
       </c>
       <c r="E39">
         <v>90000</v>
       </c>
       <c r="F39">
-        <v>0.49589800000000001</v>
+        <v>2.3074200000000001E-3</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
@@ -3563,13 +3677,13 @@
         <v>92500</v>
       </c>
       <c r="D40">
-        <v>8.7237100000000005</v>
+        <v>3.10263</v>
       </c>
       <c r="E40">
         <v>92500</v>
       </c>
       <c r="F40">
-        <v>0.49598999999999999</v>
+        <v>2.0121599999999998E-3</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.25">
@@ -3577,13 +3691,13 @@
         <v>95000</v>
       </c>
       <c r="D41">
-        <v>8.3491900000000001</v>
+        <v>2.9090099999999999</v>
       </c>
       <c r="E41">
         <v>95000</v>
       </c>
       <c r="F41">
-        <v>0.166881</v>
+        <v>2.5523500000000001E-3</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
@@ -3591,13 +3705,13 @@
         <v>97500</v>
       </c>
       <c r="D42">
-        <v>7.7038099999999998</v>
+        <v>3.0103300000000002</v>
       </c>
       <c r="E42">
         <v>97500</v>
       </c>
       <c r="F42">
-        <v>0.33084599999999997</v>
+        <v>2.5428600000000001E-3</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
@@ -3605,13 +3719,13 @@
         <v>100000</v>
       </c>
       <c r="D43">
-        <v>7.2657999999999996</v>
+        <v>2.8391199999999999</v>
       </c>
       <c r="E43">
         <v>100000</v>
       </c>
       <c r="F43">
-        <v>0.16711000000000001</v>
+        <v>2.4356500000000001E-3</v>
       </c>
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
@@ -3619,13 +3733,13 @@
         <v>102500</v>
       </c>
       <c r="D44">
-        <v>8.3569700000000005</v>
+        <v>2.90306</v>
       </c>
       <c r="E44">
         <v>102500</v>
       </c>
       <c r="F44">
-        <v>0.33131500000000003</v>
+        <v>1.6373200000000001E-3</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
@@ -3633,13 +3747,13 @@
         <v>105000</v>
       </c>
       <c r="D45">
-        <v>8.1071600000000004</v>
+        <v>2.6816900000000001</v>
       </c>
       <c r="E45">
         <v>105000</v>
       </c>
       <c r="F45">
-        <v>0.16605300000000001</v>
+        <v>1.5728599999999999E-3</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.25">
@@ -3647,13 +3761,13 @@
         <v>107500</v>
       </c>
       <c r="D46">
-        <v>7.9393500000000001</v>
+        <v>2.72397</v>
       </c>
       <c r="E46">
         <v>107500</v>
       </c>
       <c r="F46">
-        <v>0.329127</v>
+        <v>1.4586499999999999E-3</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
@@ -3661,13 +3775,13 @@
         <v>110000</v>
       </c>
       <c r="D47">
-        <v>7.6155299999999997</v>
+        <v>2.9557199999999999</v>
       </c>
       <c r="E47">
         <v>110000</v>
       </c>
       <c r="F47">
-        <v>2.2952900000000002E-3</v>
+        <v>1.61342E-3</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
@@ -3675,13 +3789,13 @@
         <v>112500</v>
       </c>
       <c r="D48">
-        <v>7.80877</v>
+        <v>2.5720000000000001</v>
       </c>
       <c r="E48">
         <v>112500</v>
       </c>
       <c r="F48">
-        <v>2.9983000000000002E-3</v>
+        <v>1.5826600000000001E-3</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
@@ -3689,13 +3803,13 @@
         <v>115000</v>
       </c>
       <c r="D49">
-        <v>6.3679800000000002</v>
+        <v>2.48515</v>
       </c>
       <c r="E49">
         <v>115000</v>
       </c>
       <c r="F49">
-        <v>0.167237</v>
+        <v>1.90087E-3</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
@@ -3703,13 +3817,13 @@
         <v>117500</v>
       </c>
       <c r="D50">
-        <v>8.12791</v>
+        <v>2.5375000000000001</v>
       </c>
       <c r="E50">
         <v>117500</v>
       </c>
       <c r="F50">
-        <v>0.16658200000000001</v>
+        <v>1.7228899999999999E-3</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.25">
@@ -3717,13 +3831,13 @@
         <v>120000</v>
       </c>
       <c r="D51">
-        <v>6.2869099999999998</v>
+        <v>2.3976899999999999</v>
       </c>
       <c r="E51">
         <v>120000</v>
       </c>
       <c r="F51">
-        <v>0.65893199999999996</v>
+        <v>1.56521E-3</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.25">
@@ -3731,13 +3845,13 @@
         <v>122500</v>
       </c>
       <c r="D52">
-        <v>7.8736699999999997</v>
+        <v>2.6780499999999998</v>
       </c>
       <c r="E52">
         <v>122500</v>
       </c>
       <c r="F52">
-        <v>0.33021699999999998</v>
+        <v>2.5086499999999999E-3</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.25">
@@ -3745,13 +3859,13 @@
         <v>125000</v>
       </c>
       <c r="D53">
-        <v>6.9713799999999999</v>
+        <v>2.5420199999999999</v>
       </c>
       <c r="E53">
         <v>125000</v>
       </c>
       <c r="F53">
-        <v>0.65660499999999999</v>
+        <v>1.92275E-3</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
@@ -3759,13 +3873,13 @@
         <v>127500</v>
       </c>
       <c r="D54">
-        <v>7.5320600000000004</v>
+        <v>2.4811999999999999</v>
       </c>
       <c r="E54">
         <v>127500</v>
       </c>
       <c r="F54">
-        <v>0.49215199999999998</v>
+        <v>1.5084E-3</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
@@ -3773,13 +3887,13 @@
         <v>130000</v>
       </c>
       <c r="D55">
-        <v>6.5980499999999997</v>
+        <v>2.3658199999999998</v>
       </c>
       <c r="E55">
         <v>130000</v>
       </c>
       <c r="F55">
-        <v>0.32714500000000002</v>
+        <v>2.24033E-3</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
@@ -3787,13 +3901,13 @@
         <v>132500</v>
       </c>
       <c r="D56">
-        <v>7.2129799999999999</v>
+        <v>2.41214</v>
       </c>
       <c r="E56">
         <v>132500</v>
       </c>
       <c r="F56">
-        <v>0.16597100000000001</v>
+        <v>2.2804499999999998E-3</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.25">
@@ -3801,13 +3915,13 @@
         <v>135000</v>
       </c>
       <c r="D57">
-        <v>7.0805899999999999</v>
+        <v>2.5205600000000001</v>
       </c>
       <c r="E57">
         <v>135000</v>
       </c>
       <c r="F57">
-        <v>0.49537700000000001</v>
+        <v>1.9222200000000001E-3</v>
       </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.25">
@@ -3815,13 +3929,13 @@
         <v>137500</v>
       </c>
       <c r="D58">
-        <v>6.7166199999999998</v>
+        <v>2.2610299999999999</v>
       </c>
       <c r="E58">
         <v>137500</v>
       </c>
       <c r="F58">
-        <v>0.65753099999999998</v>
+        <v>2.4226299999999998E-3</v>
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.25">
@@ -3829,13 +3943,13 @@
         <v>140000</v>
       </c>
       <c r="D59">
-        <v>7.6000500000000004</v>
+        <v>2.3469600000000002</v>
       </c>
       <c r="E59">
         <v>140000</v>
       </c>
       <c r="F59">
-        <v>0.33002100000000001</v>
+        <v>2.0982599999999998E-3</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
@@ -3843,13 +3957,13 @@
         <v>142500</v>
       </c>
       <c r="D60">
-        <v>7.0628900000000003</v>
+        <v>2.2210000000000001</v>
       </c>
       <c r="E60">
         <v>142500</v>
       </c>
       <c r="F60">
-        <v>0.16636500000000001</v>
+        <v>2.51447E-3</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.25">
@@ -3857,13 +3971,13 @@
         <v>145000</v>
       </c>
       <c r="D61">
-        <v>7.0819200000000002</v>
+        <v>1.9353199999999999</v>
       </c>
       <c r="E61">
         <v>145000</v>
       </c>
       <c r="F61">
-        <v>0.166239</v>
+        <v>3.1665299999999999E-3</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.25">
@@ -3871,13 +3985,13 @@
         <v>147500</v>
       </c>
       <c r="D62">
-        <v>6.9360799999999996</v>
+        <v>2.0588500000000001</v>
       </c>
       <c r="E62">
         <v>147500</v>
       </c>
       <c r="F62">
-        <v>0.16597300000000001</v>
+        <v>2.36901E-3</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
@@ -3885,13 +3999,13 @@
         <v>150000</v>
       </c>
       <c r="D63">
-        <v>6.9888899999999996</v>
+        <v>2.0888</v>
       </c>
       <c r="E63">
         <v>150000</v>
       </c>
       <c r="F63">
-        <v>0.49503799999999998</v>
+        <v>2.1789999999999999E-3</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
@@ -3899,13 +4013,13 @@
         <v>152500</v>
       </c>
       <c r="D64">
-        <v>6.2000900000000003</v>
+        <v>1.9130199999999999</v>
       </c>
       <c r="E64">
         <v>152500</v>
       </c>
       <c r="F64">
-        <v>0.65898100000000004</v>
+        <v>2.2827199999999998E-3</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
@@ -3913,13 +4027,13 @@
         <v>155000</v>
       </c>
       <c r="D65">
-        <v>6.8265399999999996</v>
+        <v>1.7782100000000001</v>
       </c>
       <c r="E65">
         <v>155000</v>
       </c>
       <c r="F65">
-        <v>0.166986</v>
+        <v>1.81237E-3</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
@@ -3927,13 +4041,13 @@
         <v>157500</v>
       </c>
       <c r="D66">
-        <v>5.1270600000000002</v>
+        <v>1.8512999999999999</v>
       </c>
       <c r="E66">
         <v>157500</v>
       </c>
       <c r="F66">
-        <v>0.49584800000000001</v>
+        <v>2.2105900000000001E-3</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
@@ -3941,13 +4055,13 @@
         <v>160000</v>
       </c>
       <c r="D67">
-        <v>6.1308499999999997</v>
+        <v>1.67974</v>
       </c>
       <c r="E67">
         <v>160000</v>
       </c>
       <c r="F67">
-        <v>0.66056099999999995</v>
+        <v>1.9303E-3</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
@@ -3955,13 +4069,13 @@
         <v>162500</v>
       </c>
       <c r="D68">
-        <v>6.2979000000000003</v>
+        <v>1.82142</v>
       </c>
       <c r="E68">
         <v>162500</v>
       </c>
       <c r="F68">
-        <v>0.330596</v>
+        <v>3.2170499999999999E-3</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
@@ -3969,13 +4083,13 @@
         <v>165000</v>
       </c>
       <c r="D69">
-        <v>6.2078199999999999</v>
+        <v>1.7111700000000001</v>
       </c>
       <c r="E69">
         <v>165000</v>
       </c>
       <c r="F69">
-        <v>1.75505E-3</v>
+        <v>3.2174299999999999E-3</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
@@ -3983,13 +4097,13 @@
         <v>167500</v>
       </c>
       <c r="D70">
-        <v>7.1746299999999996</v>
+        <v>1.85869</v>
       </c>
       <c r="E70">
         <v>167500</v>
       </c>
       <c r="F70">
-        <v>0.16536600000000001</v>
+        <v>3.24924E-3</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
@@ -3997,13 +4111,13 @@
         <v>170000</v>
       </c>
       <c r="D71">
-        <v>6.3601999999999999</v>
+        <v>1.77458</v>
       </c>
       <c r="E71">
         <v>170000</v>
       </c>
       <c r="F71">
-        <v>0.32932400000000001</v>
+        <v>2.3193300000000001E-3</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
@@ -4011,13 +4125,13 @@
         <v>172500</v>
       </c>
       <c r="D72">
-        <v>5.9301500000000003</v>
+        <v>1.64882</v>
       </c>
       <c r="E72">
         <v>172500</v>
       </c>
       <c r="F72">
-        <v>0.49462</v>
+        <v>2.5328600000000001E-3</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
@@ -4025,13 +4139,13 @@
         <v>175000</v>
       </c>
       <c r="D73">
-        <v>6.5186099999999998</v>
+        <v>1.5088999999999999</v>
       </c>
       <c r="E73">
         <v>175000</v>
       </c>
       <c r="F73">
-        <v>0.495284</v>
+        <v>2.1566799999999998E-3</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
@@ -4039,13 +4153,13 @@
         <v>177500</v>
       </c>
       <c r="D74">
-        <v>6.1236899999999999</v>
+        <v>1.5301800000000001</v>
       </c>
       <c r="E74">
         <v>177500</v>
       </c>
       <c r="F74">
-        <v>0.16603799999999999</v>
+        <v>2.3112900000000001E-3</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
@@ -4053,13 +4167,13 @@
         <v>180000</v>
       </c>
       <c r="D75">
-        <v>5.39018</v>
+        <v>1.3187899999999999</v>
       </c>
       <c r="E75">
         <v>180000</v>
       </c>
       <c r="F75">
-        <v>0.329621</v>
+        <v>1.7953999999999999E-3</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
@@ -4067,13 +4181,13 @@
         <v>182500</v>
       </c>
       <c r="D76">
-        <v>6.0289400000000004</v>
+        <v>1.4168499999999999</v>
       </c>
       <c r="E76">
         <v>182500</v>
       </c>
       <c r="F76">
-        <v>0.49267</v>
+        <v>2.25961E-3</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
@@ -4081,13 +4195,13 @@
         <v>185000</v>
       </c>
       <c r="D77">
-        <v>4.5792799999999998</v>
+        <v>1.2976099999999999</v>
       </c>
       <c r="E77">
         <v>185000</v>
       </c>
       <c r="F77">
-        <v>0.81939799999999996</v>
+        <v>1.8689100000000001E-3</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
@@ -4095,13 +4209,13 @@
         <v>187500</v>
       </c>
       <c r="D78">
-        <v>4.5284700000000004</v>
+        <v>1.28661</v>
       </c>
       <c r="E78">
         <v>187500</v>
       </c>
       <c r="F78">
-        <v>0.65917199999999998</v>
+        <v>1.90693E-3</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
@@ -4109,13 +4223,13 @@
         <v>190000</v>
       </c>
       <c r="D79">
-        <v>5.8122100000000003</v>
+        <v>1.22272</v>
       </c>
       <c r="E79">
         <v>190000</v>
       </c>
       <c r="F79">
-        <v>0.81967400000000001</v>
+        <v>2.1695E-3</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
@@ -4123,13 +4237,13 @@
         <v>192500</v>
       </c>
       <c r="D80">
-        <v>5.1693800000000003</v>
+        <v>1.2784</v>
       </c>
       <c r="E80">
         <v>192500</v>
       </c>
       <c r="F80">
-        <v>0.49275600000000003</v>
+        <v>2.1294600000000001E-3</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
@@ -4137,13 +4251,13 @@
         <v>195000</v>
       </c>
       <c r="D81">
-        <v>5.3819499999999998</v>
+        <v>1.2839</v>
       </c>
       <c r="E81">
         <v>195000</v>
       </c>
       <c r="F81">
-        <v>0.82478099999999999</v>
+        <v>1.8750699999999999E-3</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
@@ -4151,13 +4265,13 @@
         <v>197500</v>
       </c>
       <c r="D82">
-        <v>4.6578600000000003</v>
+        <v>1.18347</v>
       </c>
       <c r="E82">
         <v>197500</v>
       </c>
       <c r="F82">
-        <v>0.495305</v>
+        <v>1.8830400000000001E-3</v>
       </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.25">
@@ -4165,13 +4279,13 @@
         <v>200000</v>
       </c>
       <c r="D83">
-        <v>5.0157299999999996</v>
+        <v>1.04802</v>
       </c>
       <c r="E83">
         <v>200000</v>
       </c>
       <c r="F83">
-        <v>0.65873700000000002</v>
+        <v>1.94173E-3</v>
       </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.25">
@@ -4179,13 +4293,13 @@
         <v>202500</v>
       </c>
       <c r="D84">
-        <v>4.7200199999999999</v>
+        <v>1.05664</v>
       </c>
       <c r="E84">
         <v>202500</v>
       </c>
       <c r="F84">
-        <v>0.32969599999999999</v>
+        <v>2.0902899999999999E-3</v>
       </c>
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.25">
@@ -4193,13 +4307,13 @@
         <v>205000</v>
       </c>
       <c r="D85">
-        <v>5.7538799999999997</v>
+        <v>0.96916599999999997</v>
       </c>
       <c r="E85">
         <v>205000</v>
       </c>
       <c r="F85">
-        <v>0.49456800000000001</v>
+        <v>3.0154499999999998E-3</v>
       </c>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.25">
@@ -4207,13 +4321,13 @@
         <v>207500</v>
       </c>
       <c r="D86">
-        <v>4.8214100000000002</v>
+        <v>0.96930899999999998</v>
       </c>
       <c r="E86">
         <v>207500</v>
       </c>
       <c r="F86">
-        <v>0.33023000000000002</v>
+        <v>1.85227E-3</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
@@ -4221,13 +4335,13 @@
         <v>210000</v>
       </c>
       <c r="D87">
-        <v>4.0613299999999999</v>
+        <v>0.90728799999999998</v>
       </c>
       <c r="E87">
         <v>210000</v>
       </c>
       <c r="F87">
-        <v>0.49491099999999999</v>
+        <v>1.81492E-3</v>
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
@@ -4235,13 +4349,13 @@
         <v>212500</v>
       </c>
       <c r="D88">
-        <v>5.0863199999999997</v>
+        <v>0.83740199999999998</v>
       </c>
       <c r="E88">
         <v>212500</v>
       </c>
       <c r="F88">
-        <v>0.33126299999999997</v>
+        <v>2.1383399999999999E-3</v>
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
@@ -4249,13 +4363,13 @@
         <v>215000</v>
       </c>
       <c r="D89">
-        <v>3.9412799999999999</v>
+        <v>0.80911200000000005</v>
       </c>
       <c r="E89">
         <v>215000</v>
       </c>
       <c r="F89">
-        <v>0.33006999999999997</v>
+        <v>3.6200799999999999E-3</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.25">
@@ -4263,13 +4377,13 @@
         <v>217500</v>
       </c>
       <c r="D90">
-        <v>4.2573699999999999</v>
+        <v>0.66082200000000002</v>
       </c>
       <c r="E90">
         <v>217500</v>
       </c>
       <c r="F90">
-        <v>0.328851</v>
+        <v>3.4783399999999999E-3</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">
@@ -4277,13 +4391,13 @@
         <v>220000</v>
       </c>
       <c r="D91">
-        <v>4.5664999999999996</v>
+        <v>0.65816300000000005</v>
       </c>
       <c r="E91">
         <v>220000</v>
       </c>
       <c r="F91">
-        <v>0.329291</v>
+        <v>3.00038E-3</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.25">
@@ -4291,13 +4405,13 @@
         <v>222500</v>
       </c>
       <c r="D92">
-        <v>2.9846699999999999</v>
+        <v>0.665107</v>
       </c>
       <c r="E92">
         <v>222500</v>
       </c>
       <c r="F92">
-        <v>0.49656600000000001</v>
+        <v>2.2781799999999999E-3</v>
       </c>
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.25">
@@ -4305,13 +4419,13 @@
         <v>225000</v>
       </c>
       <c r="D93">
-        <v>4.2580799999999996</v>
+        <v>0.65404200000000001</v>
       </c>
       <c r="E93">
         <v>225000</v>
       </c>
       <c r="F93">
-        <v>0.16579199999999999</v>
+        <v>3.8428799999999999E-3</v>
       </c>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.25">
@@ -4319,13 +4433,13 @@
         <v>227500</v>
       </c>
       <c r="D94">
-        <v>3.9935299999999998</v>
+        <v>0.599074</v>
       </c>
       <c r="E94">
         <v>227500</v>
       </c>
       <c r="F94">
-        <v>0.330507</v>
+        <v>4.5530900000000001E-3</v>
       </c>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.25">
@@ -4333,13 +4447,13 @@
         <v>230000</v>
       </c>
       <c r="D95">
-        <v>3.2849699999999999</v>
+        <v>0.53460099999999999</v>
       </c>
       <c r="E95">
         <v>230000</v>
       </c>
       <c r="F95">
-        <v>0.65519099999999997</v>
+        <v>2.6874500000000001E-3</v>
       </c>
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.25">
@@ -4347,13 +4461,13 @@
         <v>232500</v>
       </c>
       <c r="D96">
-        <v>3.2231200000000002</v>
+        <v>0.51446999999999998</v>
       </c>
       <c r="E96">
         <v>232500</v>
       </c>
       <c r="F96">
-        <v>0.327984</v>
+        <v>3.01308E-3</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.25">
@@ -4361,13 +4475,13 @@
         <v>235000</v>
       </c>
       <c r="D97">
-        <v>4.5000499999999999</v>
+        <v>0.485211</v>
       </c>
       <c r="E97">
         <v>235000</v>
       </c>
       <c r="F97">
-        <v>0.32834600000000003</v>
+        <v>2.4972800000000002E-3</v>
       </c>
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.25">
@@ -4375,13 +4489,13 @@
         <v>237500</v>
       </c>
       <c r="D98">
-        <v>4.3731499999999999</v>
+        <v>0.46825600000000001</v>
       </c>
       <c r="E98">
         <v>237500</v>
       </c>
       <c r="F98">
-        <v>0.32916499999999999</v>
+        <v>2.1240199999999999E-3</v>
       </c>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.25">
@@ -4389,13 +4503,13 @@
         <v>240000</v>
       </c>
       <c r="D99">
-        <v>3.1986400000000001</v>
+        <v>0.45920100000000003</v>
       </c>
       <c r="E99">
         <v>240000</v>
       </c>
       <c r="F99">
-        <v>0.49386400000000003</v>
+        <v>2.0739600000000001E-3</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
@@ -4403,13 +4517,13 @@
         <v>242500</v>
       </c>
       <c r="D100">
-        <v>2.5594399999999999</v>
+        <v>0.43281799999999998</v>
       </c>
       <c r="E100">
         <v>242500</v>
       </c>
       <c r="F100">
-        <v>0.49198599999999998</v>
+        <v>2.3248100000000001E-3</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
@@ -4417,13 +4531,13 @@
         <v>245000</v>
       </c>
       <c r="D101">
-        <v>2.6231599999999999</v>
+        <v>0.42285400000000001</v>
       </c>
       <c r="E101">
         <v>245000</v>
       </c>
       <c r="F101">
-        <v>0.165939</v>
+        <v>2.6210199999999999E-3</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
@@ -4431,13 +4545,13 @@
         <v>247500</v>
       </c>
       <c r="D102">
-        <v>3.82626</v>
+        <v>0.432861</v>
       </c>
       <c r="E102">
         <v>247500</v>
       </c>
       <c r="F102">
-        <v>0.330571</v>
+        <v>3.06558E-3</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.25">
@@ -4445,13 +4559,13 @@
         <v>250000</v>
       </c>
       <c r="D103">
-        <v>3.7863099999999998</v>
+        <v>0.38176700000000002</v>
       </c>
       <c r="E103">
         <v>250000</v>
       </c>
       <c r="F103">
-        <v>0.16677500000000001</v>
+        <v>3.01951E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>